<commit_message>
finalized prototype, just clean-up stuff
</commit_message>
<xml_diff>
--- a/data/urls/urls-categorized_0.3-10122017.xlsx
+++ b/data/urls/urls-categorized_0.3-10122017.xlsx
@@ -912,21 +912,21 @@
   </sheetPr>
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="50.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="10.69"/>
   </cols>
   <sheetData>
@@ -1711,7 +1711,7 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>